<commit_message>
Clean up demo forms
</commit_message>
<xml_diff>
--- a/demo-forms/enketo_widgets/forms/app/enketo_widgets.xlsx
+++ b/demo-forms/enketo_widgets/forms/app/enketo_widgets.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="375">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -95,8 +95,7 @@
   </si>
   <si>
     <t xml:space="preserve">This form showcases the different available _widgets_. 
-The hints explain how these widgets were created. The form logo was added by simply uploading a file called *form_logo.png* as part of the form media.
-The XLS Form source is [here](https://docs.google.com/spreadsheet/ccc?key=0Al3Mw5sknZoPdEpPa29tamFCc1o2bmFVR3RaemlSRXc&amp;usp=sharing).</t>
+The hints explain how these widgets were created.</t>
   </si>
   <si>
     <t xml:space="preserve">begin_group</t>
@@ -764,33 +763,6 @@
   </si>
   <si>
     <t xml:space="preserve">Select an image or take a photo (type=image)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">draw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Draw widget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make a drawing (type=image, appearance=draw)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signature widget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add a signature (type=image, appearance=signature)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annotate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annotate image widget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upload and annotate an image (type=image, appearance=annotate)</t>
   </si>
   <si>
     <t xml:space="preserve">audio</t>
@@ -1447,12 +1419,12 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="C84" activeCellId="0" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.29"/>
@@ -3239,7 +3211,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
@@ -3251,9 +3223,7 @@
       <c r="E76" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>238</v>
-      </c>
+      <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -3264,7 +3234,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
@@ -3276,9 +3246,7 @@
       <c r="E77" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>241</v>
-      </c>
+      <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -3287,9 +3255,9 @@
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
@@ -3301,9 +3269,7 @@
       <c r="E78" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>244</v>
-      </c>
+      <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3312,20 +3278,14 @@
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>247</v>
+        <v>38</v>
       </c>
       <c r="B79" s="2"/>
-      <c r="C79" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>249</v>
-      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3335,42 +3295,42 @@
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-    </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>253</v>
+        <v>13</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -3379,16 +3339,24 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
-      <c r="M81" s="2"/>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M81" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -3398,57 +3366,53 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3" t="s">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="E83" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D84" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>260</v>
-      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L84" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
@@ -3469,20 +3433,14 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>264</v>
+        <v>38</v>
       </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>266</v>
-      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -3491,67 +3449,6 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
-    </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="M87" s="2"/>
-    </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-      <c r="L88" s="2"/>
-      <c r="M88" s="2"/>
-    </row>
-    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="2"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3576,11 +3473,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
@@ -3591,7 +3488,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>2</v>
@@ -3600,7 +3497,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>194</v>
@@ -3619,13 +3516,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3633,13 +3530,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3647,13 +3544,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -3661,13 +3558,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -3683,48 +3580,48 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>284</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>293</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -3739,13 +3636,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -3753,13 +3650,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3767,13 +3664,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B14" s="9" t="n">
         <v>3</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -3781,13 +3678,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -3795,13 +3692,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>5</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -3809,13 +3706,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -3823,13 +3720,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -3837,13 +3734,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -3859,13 +3756,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -3873,13 +3770,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -3887,13 +3784,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -3901,13 +3798,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -3923,13 +3820,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -3937,13 +3834,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -3951,13 +3848,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B28" s="9" t="n">
         <v>3</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -3965,13 +3862,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B29" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -3979,13 +3876,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B30" s="9" t="n">
         <v>5</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -4001,13 +3898,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -4015,13 +3912,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -4029,13 +3926,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -4043,13 +3940,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -4057,13 +3954,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -4071,13 +3968,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -4093,32 +3990,32 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -4133,64 +4030,64 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
@@ -4205,32 +4102,32 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -4245,13 +4142,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -4259,13 +4156,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -4281,97 +4178,97 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="B57" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>351</v>
-      </c>
       <c r="C57" s="9" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F58" s="9"/>
     </row>
@@ -4385,164 +4282,164 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="F62" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="B64" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>364</v>
-      </c>
       <c r="C64" s="9" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4634,7 +4531,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
@@ -4643,43 +4540,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="C2" s="10" t="n">
         <f aca="true">TODAY()</f>
-        <v>44453</v>
+        <v>44460</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More cleanup on the demo form add proper public domain images
</commit_message>
<xml_diff>
--- a/demo-forms/enketo_widgets/forms/app/enketo_widgets.xlsx
+++ b/demo-forms/enketo_widgets/forms/app/enketo_widgets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="K23" authorId="0">
+    <comment ref="K22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="371">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">intro</t>
   </si>
   <si>
-    <t xml:space="preserve">This form showcases the different available _widgets_. 
+    <t xml:space="preserve">This form showcases the different available Enketo _widgets_. 
 The hints explain how these widgets were created.</t>
   </si>
   <si>
@@ -141,15 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">multiline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barcode widget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scans multi-format 1d/2d barcodes. In enketo it allows manual entry (type=barcode)</t>
   </si>
   <si>
     <t xml:space="preserve">url</t>
@@ -513,7 +504,7 @@
     <t xml:space="preserve">No buttons</t>
   </si>
   <si>
-    <t xml:space="preserve">Make sure to put a.jpg and b.jpg in the form-media folder to see images here. (type=select_one, appearance=no-buttons)</t>
+    <t xml:space="preserve">Make sure to put a.png and b.png in the impages folder to see images here. (type=select_one, appearance=no-buttons)</t>
   </si>
   <si>
     <t xml:space="preserve">no-buttons</t>
@@ -1005,9 +996,6 @@
   </si>
   <si>
     <t xml:space="preserve">a_b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO_LABEL</t>
   </si>
   <si>
     <t xml:space="preserve">a.png</t>
@@ -1418,13 +1406,13 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C84" activeCellId="0" sqref="C84"/>
+      <selection pane="bottomLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.29"/>
@@ -1601,7 +1589,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -1610,200 +1598,204 @@
       <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="K7" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>18.31</v>
+      </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>18.31</v>
-      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="D14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>58</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="5" t="s">
         <v>60</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1815,22 +1807,22 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1842,22 +1834,22 @@
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1869,22 +1861,22 @@
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1895,23 +1887,21 @@
       <c r="M18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="D19" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="E19" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1923,21 +1913,13 @@
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1947,86 +1929,94 @@
       <c r="M20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="6" t="s">
-        <v>86</v>
-      </c>
+      <c r="K23" s="6"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2038,26 +2028,24 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="6"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
@@ -2067,13 +2055,13 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2086,18 +2074,12 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2108,92 +2090,100 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+      <c r="A28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="E29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2203,22 +2193,22 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2228,72 +2218,72 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="K33" s="2" t="n">
+        <v>8</v>
+      </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2" t="n">
-        <v>8</v>
-      </c>
+      <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2305,20 +2295,20 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2330,20 +2320,20 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2353,22 +2343,22 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2378,22 +2368,22 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2403,22 +2393,22 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2428,70 +2418,70 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D41" s="2" t="s">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="D41" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7" t="s">
+      <c r="D42" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="F42" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
         <v>163</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2503,20 +2493,20 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2526,23 +2516,15 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>169</v>
-      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -2552,58 +2534,64 @@
       <c r="M45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7" t="s">
+      <c r="A47" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -2616,18 +2604,12 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>178</v>
-      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2638,58 +2620,64 @@
       <c r="M49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
+      <c r="A50" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7" t="s">
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
+      <c r="E51" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -2700,20 +2688,14 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -2725,7 +2707,7 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>172</v>
+        <v>35</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2741,65 +2723,69 @@
       <c r="M54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+      <c r="A55" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7" t="s">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
@@ -2812,9 +2798,13 @@
       <c r="D58" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+      <c r="G58" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -2824,21 +2814,21 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2849,22 +2839,14 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>201</v>
+        <v>35</v>
       </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>204</v>
-      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="2" t="s">
-        <v>205</v>
-      </c>
+      <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -2873,61 +2855,71 @@
       <c r="M60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
+      <c r="A61" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7" t="s">
+      <c r="A62" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="7"/>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F62" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>195</v>
       </c>
       <c r="E63" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -2937,20 +2929,20 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
         <v>210</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>211</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>212</v>
@@ -2962,26 +2954,16 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>201</v>
+        <v>35</v>
       </c>
       <c r="B65" s="2"/>
-      <c r="C65" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>215</v>
-      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -2991,7 +2973,7 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3006,62 +2988,70 @@
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3" t="s">
+      <c r="A68" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E68" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -3073,20 +3063,20 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -3111,7 +3101,7 @@
         <v>229</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -3123,21 +3113,13 @@
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>230</v>
+        <v>35</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -3147,44 +3129,50 @@
       <c r="M72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-    </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
+      <c r="A73" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3" t="s">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="E74" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
@@ -3232,7 +3220,7 @@
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>241</v>
       </c>
@@ -3257,18 +3245,12 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>244</v>
+        <v>35</v>
       </c>
       <c r="B78" s="2"/>
-      <c r="C78" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>246</v>
-      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -3279,48 +3261,56 @@
       <c r="M78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-    </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+      <c r="A79" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3" t="s">
+      <c r="B79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="E80" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
@@ -3339,13 +3329,11 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
-      <c r="M81" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="M81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>146</v>
+        <v>252</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
@@ -3366,64 +3354,58 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D83" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>257</v>
-      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
-      <c r="L83" s="2"/>
+      <c r="L83" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="M83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>258</v>
+        <v>13</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+      <c r="E84" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
-      <c r="L84" s="2" t="s">
-        <v>260</v>
-      </c>
+      <c r="L84" s="2"/>
       <c r="M84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>263</v>
-      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -3433,27 +3415,10 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId2" display="https://enketo.org"/>
+    <hyperlink ref="K7" r:id="rId2" display="https://enketo.org"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3473,22 +3438,23 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>2</v>
@@ -3497,13 +3463,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,13 +3482,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3530,13 +3496,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>269</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -3544,13 +3510,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -3558,13 +3524,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -3580,48 +3546,48 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>275</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>278</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -3636,13 +3602,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -3650,13 +3616,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3664,13 +3630,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B14" s="9" t="n">
         <v>3</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -3678,13 +3644,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -3692,13 +3658,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>5</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -3706,13 +3672,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -3720,13 +3686,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -3734,13 +3700,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -3756,13 +3722,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -3770,13 +3736,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>294</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>297</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -3784,13 +3750,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -3798,13 +3764,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -3820,13 +3786,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -3834,13 +3800,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -3848,13 +3814,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B28" s="9" t="n">
         <v>3</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -3862,13 +3828,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B29" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -3876,13 +3842,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B30" s="9" t="n">
         <v>5</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -3898,13 +3864,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -3912,13 +3878,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -3926,13 +3892,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>308</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>311</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -3940,13 +3906,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -3954,13 +3920,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -3968,13 +3934,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -3990,37 +3956,33 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>318</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C39" s="9"/>
       <c r="D39" s="9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>318</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="C40" s="9"/>
       <c r="D40" s="9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -4030,69 +3992,61 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>318</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C42" s="9"/>
       <c r="D42" s="9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>318</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="C43" s="9"/>
       <c r="D43" s="9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="C44" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
         <v>318</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>322</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>318</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -4102,32 +4056,28 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>318</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="C47" s="9"/>
       <c r="D47" s="9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9" t="s">
         <v>324</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>328</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -4142,13 +4092,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -4156,13 +4106,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -4178,97 +4128,97 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>337</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F58" s="9"/>
     </row>
@@ -4282,164 +4232,164 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>346</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>350</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>330</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>330</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4531,7 +4481,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
@@ -4540,43 +4490,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C2" s="10" t="n">
         <f aca="true">TODAY()</f>
         <v>44460</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>